<commit_message>
Fix character encoding for vívoactive / vívomove
</commit_message>
<xml_diff>
--- a/data/gp3s-devices-options.xlsx
+++ b/data/gp3s-devices-options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mike\projects\work\gp3s-query\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06BBA66-3F2C-4F71-964D-386991261376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388B5D2E-FFDF-4F94-865D-BF056C5C3A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4CB867C2-8EB5-4F35-9DD0-5D686A7A8D37}"/>
   </bookViews>
@@ -617,24 +617,9 @@
     <t>Garmin Venu 2 Plus</t>
   </si>
   <si>
-    <t>Garmin v&amp;#237;voactive 3</t>
-  </si>
-  <si>
     <t>Garmin vivoactive 3 Music</t>
   </si>
   <si>
-    <t>Garmin v&amp;#237;voactive 4</t>
-  </si>
-  <si>
-    <t>Garmin v&amp;#237;voactive 4S</t>
-  </si>
-  <si>
-    <t>Garmin v&amp;#237;voactive 5</t>
-  </si>
-  <si>
-    <t>Garmin v&amp;#237;voactive HR</t>
-  </si>
-  <si>
     <t>Garmin vivoactive3</t>
   </si>
   <si>
@@ -650,9 +635,6 @@
     <t>Garmin vivoactiveHR</t>
   </si>
   <si>
-    <t>Garmin v&amp;#237;vomove Style</t>
-  </si>
-  <si>
     <t>Garmin vivosmartHR+</t>
   </si>
   <si>
@@ -1326,6 +1308,24 @@
   </si>
   <si>
     <t>Forerunner 735XT</t>
+  </si>
+  <si>
+    <t>Garmin vívoactive HR</t>
+  </si>
+  <si>
+    <t>Garmin vívoactive 3</t>
+  </si>
+  <si>
+    <t>Garmin vívoactive 4</t>
+  </si>
+  <si>
+    <t>Garmin vívoactive 4S</t>
+  </si>
+  <si>
+    <t>Garmin vívoactive 5</t>
+  </si>
+  <si>
+    <t>Garmin vívomove Style</t>
   </si>
 </sst>
 </file>
@@ -1713,8 +1713,8 @@
   <dimension ref="A1:F249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A217" sqref="A217"/>
+      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A194" sqref="A194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,22 +1729,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1752,27 +1752,27 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1780,13 +1780,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1794,13 +1794,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1811,10 +1811,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1822,13 +1822,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1836,13 +1836,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1850,13 +1850,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1864,13 +1864,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1878,13 +1878,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1892,13 +1892,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1906,13 +1906,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1920,13 +1920,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1934,13 +1934,13 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1948,13 +1948,13 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1962,13 +1962,13 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1979,10 +1979,10 @@
         <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1993,13 +1993,13 @@
         <v>23</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2010,10 +2010,10 @@
         <v>23</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2024,10 +2024,10 @@
         <v>23</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2038,10 +2038,10 @@
         <v>23</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2052,10 +2052,10 @@
         <v>23</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2066,10 +2066,10 @@
         <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2080,13 +2080,13 @@
         <v>23</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2097,10 +2097,10 @@
         <v>23</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2111,24 +2111,24 @@
         <v>23</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2139,10 +2139,10 @@
         <v>23</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2153,10 +2153,10 @@
         <v>23</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2167,10 +2167,10 @@
         <v>23</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2181,10 +2181,10 @@
         <v>23</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2195,13 +2195,13 @@
         <v>23</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="E33" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2212,13 +2212,13 @@
         <v>23</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="E34" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2229,10 +2229,10 @@
         <v>23</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2243,10 +2243,10 @@
         <v>23</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2257,10 +2257,10 @@
         <v>23</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2271,10 +2271,10 @@
         <v>23</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2285,10 +2285,10 @@
         <v>23</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2299,10 +2299,10 @@
         <v>23</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2313,10 +2313,10 @@
         <v>23</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2327,10 +2327,10 @@
         <v>23</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2341,13 +2341,13 @@
         <v>23</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="E43" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2358,13 +2358,13 @@
         <v>23</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="E44" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2375,10 +2375,10 @@
         <v>23</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2389,10 +2389,10 @@
         <v>23</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2403,10 +2403,10 @@
         <v>23</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2417,13 +2417,13 @@
         <v>23</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E48" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2434,10 +2434,10 @@
         <v>23</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2448,13 +2448,13 @@
         <v>23</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E50" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2465,13 +2465,13 @@
         <v>23</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E51" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2482,13 +2482,13 @@
         <v>23</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E52" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2499,13 +2499,13 @@
         <v>23</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E53" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2516,10 +2516,10 @@
         <v>23</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2530,10 +2530,10 @@
         <v>23</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2544,10 +2544,10 @@
         <v>23</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2558,10 +2558,10 @@
         <v>23</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2572,10 +2572,10 @@
         <v>23</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2586,13 +2586,13 @@
         <v>23</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="E59" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2603,10 +2603,10 @@
         <v>23</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2617,13 +2617,13 @@
         <v>23</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="E61" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2634,10 +2634,10 @@
         <v>23</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2648,10 +2648,10 @@
         <v>23</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2662,10 +2662,10 @@
         <v>23</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2676,10 +2676,10 @@
         <v>23</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2690,10 +2690,10 @@
         <v>23</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2704,10 +2704,10 @@
         <v>23</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2718,10 +2718,10 @@
         <v>23</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2732,10 +2732,10 @@
         <v>23</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2746,13 +2746,13 @@
         <v>23</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E70" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2763,13 +2763,13 @@
         <v>23</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E71" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2780,13 +2780,13 @@
         <v>23</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E72" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2797,13 +2797,13 @@
         <v>23</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E73" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2814,13 +2814,13 @@
         <v>23</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E74" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2831,13 +2831,13 @@
         <v>23</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E75" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2848,13 +2848,13 @@
         <v>23</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E76" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2865,10 +2865,10 @@
         <v>23</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2879,10 +2879,10 @@
         <v>23</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2893,10 +2893,10 @@
         <v>23</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2907,13 +2907,13 @@
         <v>23</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="E80" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2924,10 +2924,10 @@
         <v>23</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2938,10 +2938,10 @@
         <v>23</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2952,13 +2952,13 @@
         <v>23</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="E83" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2969,13 +2969,13 @@
         <v>23</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="E84" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2986,13 +2986,13 @@
         <v>23</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="E85" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3003,10 +3003,10 @@
         <v>23</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3017,13 +3017,13 @@
         <v>23</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E87" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3034,13 +3034,13 @@
         <v>23</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E88" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3051,13 +3051,13 @@
         <v>23</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E89" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3068,13 +3068,13 @@
         <v>23</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E90" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3085,13 +3085,13 @@
         <v>23</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E91" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3102,13 +3102,13 @@
         <v>23</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E92" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3119,13 +3119,13 @@
         <v>23</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E93" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3136,10 +3136,10 @@
         <v>23</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3150,13 +3150,13 @@
         <v>23</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="E95" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3167,13 +3167,13 @@
         <v>23</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="E96" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3184,13 +3184,13 @@
         <v>23</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="E97" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3201,10 +3201,10 @@
         <v>23</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3215,13 +3215,13 @@
         <v>23</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="E99" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3232,10 +3232,10 @@
         <v>23</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3246,13 +3246,13 @@
         <v>23</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="E101" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3263,13 +3263,13 @@
         <v>23</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="E102" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3280,10 +3280,10 @@
         <v>23</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3294,13 +3294,13 @@
         <v>23</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E104" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3311,13 +3311,13 @@
         <v>23</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E105" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3328,13 +3328,13 @@
         <v>23</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E106" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3345,13 +3345,13 @@
         <v>23</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E107" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3362,13 +3362,13 @@
         <v>23</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E108" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3379,10 +3379,10 @@
         <v>23</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="110" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3393,10 +3393,10 @@
         <v>23</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
     </row>
     <row r="111" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3407,10 +3407,10 @@
         <v>23</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
     </row>
     <row r="112" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3421,10 +3421,10 @@
         <v>23</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
     </row>
     <row r="113" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3435,10 +3435,10 @@
         <v>23</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3449,10 +3449,10 @@
         <v>23</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3463,10 +3463,10 @@
         <v>23</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3477,13 +3477,13 @@
         <v>23</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E116" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3494,13 +3494,13 @@
         <v>23</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E117" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3511,10 +3511,10 @@
         <v>23</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3525,10 +3525,10 @@
         <v>23</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3539,13 +3539,13 @@
         <v>23</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E120" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3556,13 +3556,13 @@
         <v>23</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E121" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3573,10 +3573,10 @@
         <v>23</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -3587,10 +3587,10 @@
         <v>23</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -3601,10 +3601,10 @@
         <v>23</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -3615,10 +3615,10 @@
         <v>23</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -3629,10 +3629,10 @@
         <v>23</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -3643,10 +3643,10 @@
         <v>23</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3657,10 +3657,10 @@
         <v>23</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -3671,10 +3671,10 @@
         <v>23</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -3685,10 +3685,10 @@
         <v>23</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3699,10 +3699,10 @@
         <v>23</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -3713,10 +3713,10 @@
         <v>23</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -3727,10 +3727,10 @@
         <v>23</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3741,13 +3741,13 @@
         <v>23</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E134" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3758,13 +3758,13 @@
         <v>23</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E135" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3775,10 +3775,10 @@
         <v>23</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3789,10 +3789,10 @@
         <v>23</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3803,10 +3803,10 @@
         <v>23</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3817,24 +3817,24 @@
         <v>23</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="B140" t="s">
         <v>23</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -3845,10 +3845,10 @@
         <v>23</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3859,10 +3859,10 @@
         <v>23</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -3873,10 +3873,10 @@
         <v>23</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -3887,10 +3887,10 @@
         <v>23</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -3901,10 +3901,10 @@
         <v>23</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -3915,10 +3915,10 @@
         <v>23</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -3929,13 +3929,13 @@
         <v>23</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E147" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -3946,13 +3946,13 @@
         <v>23</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E148" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -3963,10 +3963,10 @@
         <v>23</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -3977,10 +3977,10 @@
         <v>23</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -3991,10 +3991,10 @@
         <v>23</v>
       </c>
       <c r="C151" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D151" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="152" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4005,10 +4005,10 @@
         <v>23</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="153" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4019,10 +4019,10 @@
         <v>23</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="154" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4033,10 +4033,10 @@
         <v>23</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="155" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4047,10 +4047,10 @@
         <v>23</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4061,13 +4061,13 @@
         <v>23</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="E156" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4078,13 +4078,13 @@
         <v>23</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="E157" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -4095,13 +4095,13 @@
         <v>23</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="E158" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4112,13 +4112,13 @@
         <v>23</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="E159" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4129,13 +4129,13 @@
         <v>23</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="E160" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4146,13 +4146,13 @@
         <v>23</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="E161" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4163,13 +4163,13 @@
         <v>23</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="E162" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -4180,10 +4180,10 @@
         <v>23</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4194,13 +4194,13 @@
         <v>23</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="E164" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -4211,13 +4211,13 @@
         <v>23</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="E165" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -4228,13 +4228,13 @@
         <v>23</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="E166" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -4245,10 +4245,10 @@
         <v>23</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -4259,13 +4259,13 @@
         <v>23</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="E168" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -4276,13 +4276,13 @@
         <v>23</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="E169" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -4293,13 +4293,13 @@
         <v>23</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="E170" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -4310,10 +4310,10 @@
         <v>23</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -4324,13 +4324,13 @@
         <v>23</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="E172" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4341,13 +4341,13 @@
         <v>23</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="E173" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4358,10 +4358,10 @@
         <v>23</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="175" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4372,10 +4372,10 @@
         <v>23</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
     <row r="176" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4386,10 +4386,10 @@
         <v>23</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="177" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4400,10 +4400,10 @@
         <v>23</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -4414,10 +4414,10 @@
         <v>23</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -4428,13 +4428,13 @@
         <v>23</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="E179" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
@@ -4445,10 +4445,10 @@
         <v>23</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -4459,13 +4459,13 @@
         <v>23</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="E181" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
@@ -4476,10 +4476,10 @@
         <v>23</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
@@ -4490,10 +4490,10 @@
         <v>23</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
@@ -4504,13 +4504,13 @@
         <v>23</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="E184" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
@@ -4521,13 +4521,13 @@
         <v>23</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="E185" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
@@ -4538,10 +4538,10 @@
         <v>23</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
@@ -4552,13 +4552,13 @@
         <v>23</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="E187" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="188" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4569,13 +4569,13 @@
         <v>23</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="F188" s="2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
@@ -4586,10 +4586,10 @@
         <v>23</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
@@ -4600,10 +4600,10 @@
         <v>23</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
@@ -4614,10 +4614,10 @@
         <v>23</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
@@ -4628,13 +4628,13 @@
         <v>23</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="E192" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="193" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4645,10 +4645,10 @@
         <v>23</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
     </row>
     <row r="194" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4659,10 +4659,10 @@
         <v>23</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="195" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4673,210 +4673,210 @@
         <v>23</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>197</v>
+        <v>423</v>
       </c>
       <c r="B196" t="s">
         <v>23</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="E196" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B197" t="s">
         <v>23</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="E197" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B198" t="s">
         <v>23</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="E198" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B199" t="s">
         <v>23</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="E199" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>192</v>
+        <v>424</v>
       </c>
       <c r="B200" t="s">
         <v>23</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B201" t="s">
         <v>23</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>194</v>
+        <v>425</v>
       </c>
       <c r="B202" t="s">
         <v>23</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B203" t="s">
         <v>23</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>195</v>
+        <v>426</v>
       </c>
       <c r="B204" t="s">
         <v>23</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B205" t="s">
         <v>23</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>196</v>
+        <v>427</v>
       </c>
       <c r="B206" t="s">
         <v>23</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="207" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>203</v>
+        <v>428</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="E207" s="2" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="208" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B208" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="E208" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -4887,10 +4887,10 @@
         <v>23</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -4901,592 +4901,592 @@
         <v>23</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B211" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B212" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B213" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B214" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B215" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B216" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B217" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B218" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B219" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B220" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B221" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B222" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="E222" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B223" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B224" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B225" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="E225" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B226" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="E226" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B227" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B228" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B229" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B230" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B231" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="E231" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B232" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="E232" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B233" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B234" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="E234" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B235" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="E235" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B236" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="E236" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="237" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="F237" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="238" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C238" s="3" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="D238" s="3" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B239" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="E239" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B240" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B241" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="E241" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B242" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
     </row>
     <row r="243" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C243" s="3" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D243" s="3" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="E243" s="2" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B244" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B245" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B246" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B247" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B248" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B249" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>